<commit_message>
Adding dropout model data
</commit_message>
<xml_diff>
--- a/excel/exp1acc.xlsx
+++ b/excel/exp1acc.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Frequently Used\Fall 2015\CS760\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\public\food-image-classification\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="acc2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -575,7 +575,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -975,7 +975,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-03C3-4EC6-9D72-3872BC5188B5}"/>
             </c:ext>
@@ -1362,7 +1362,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-03C3-4EC6-9D72-3872BC5188B5}"/>
             </c:ext>
@@ -1749,7 +1749,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-03C3-4EC6-9D72-3872BC5188B5}"/>
             </c:ext>
@@ -2136,7 +2136,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-03C3-4EC6-9D72-3872BC5188B5}"/>
             </c:ext>
@@ -2150,11 +2150,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="471492224"/>
-        <c:axId val="471492880"/>
+        <c:axId val="303759744"/>
+        <c:axId val="303760304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="471492224"/>
+        <c:axId val="303759744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="55"/>
@@ -2175,6 +2175,20 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -2268,13 +2282,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="471492880"/>
+        <c:crossAx val="303760304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="471492880"/>
+        <c:axId val="303760304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2294,6 +2308,20 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -2392,7 +2420,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="471492224"/>
+        <c:crossAx val="303759744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3033,16 +3061,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>131445</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>80010</xdr:rowOff>
+      <xdr:rowOff>165735</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>346710</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>51435</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>70485</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3330,12 +3358,12 @@
   <dimension ref="A1:I110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3361,7 +3389,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.15624997019799999</v>
       </c>
@@ -3378,23 +3406,23 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <f>A2*100</f>
+        <f t="shared" ref="F2:F33" si="0">A2*100</f>
         <v>15.624997019799999</v>
       </c>
       <c r="G2">
-        <f>B2*100</f>
+        <f t="shared" ref="G2:G33" si="1">B2*100</f>
         <v>23.824997246300001</v>
       </c>
       <c r="H2">
-        <f>C2*100</f>
+        <f t="shared" ref="H2:H33" si="2">C2*100</f>
         <v>23.649998009199997</v>
       </c>
       <c r="I2">
-        <f>D2*100</f>
+        <f t="shared" ref="I2:I33" si="3">D2*100</f>
         <v>27.750000357600001</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.14024998247600001</v>
       </c>
@@ -3411,23 +3439,23 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <f>A3*100</f>
+        <f t="shared" si="0"/>
         <v>14.024998247600001</v>
       </c>
       <c r="G3">
-        <f>B3*100</f>
+        <f t="shared" si="1"/>
         <v>17.399999499300002</v>
       </c>
       <c r="H3">
-        <f>C3*100</f>
+        <f t="shared" si="2"/>
         <v>13.0750000477</v>
       </c>
       <c r="I3">
-        <f>D3*100</f>
+        <f t="shared" si="3"/>
         <v>18.875001370899998</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.12999999523200001</v>
       </c>
@@ -3444,23 +3472,23 @@
         <v>3</v>
       </c>
       <c r="F4">
-        <f>A4*100</f>
+        <f t="shared" si="0"/>
         <v>12.999999523200001</v>
       </c>
       <c r="G4">
-        <f>B4*100</f>
+        <f t="shared" si="1"/>
         <v>12.624999880800001</v>
       </c>
       <c r="H4">
-        <f>C4*100</f>
+        <f t="shared" si="2"/>
         <v>10.974999517200001</v>
       </c>
       <c r="I4">
-        <f>D4*100</f>
+        <f t="shared" si="3"/>
         <v>15.549997985399999</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.121500000358</v>
       </c>
@@ -3477,23 +3505,23 @@
         <v>4</v>
       </c>
       <c r="F5">
-        <f>A5*100</f>
+        <f t="shared" si="0"/>
         <v>12.1500000358</v>
       </c>
       <c r="G5">
-        <f>B5*100</f>
+        <f t="shared" si="1"/>
         <v>10.5999998748</v>
       </c>
       <c r="H5">
-        <f>C5*100</f>
+        <f t="shared" si="2"/>
         <v>11.3000005484</v>
       </c>
       <c r="I5">
-        <f>D5*100</f>
+        <f t="shared" si="3"/>
         <v>13.149999082100001</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.114500023425</v>
       </c>
@@ -3510,23 +3538,23 @@
         <v>5</v>
       </c>
       <c r="F6">
-        <f>A6*100</f>
+        <f t="shared" si="0"/>
         <v>11.450002342499999</v>
       </c>
       <c r="G6">
-        <f>B6*100</f>
+        <f t="shared" si="1"/>
         <v>9.5249995589300003</v>
       </c>
       <c r="H6">
-        <f>C6*100</f>
+        <f t="shared" si="2"/>
         <v>10.274998843700001</v>
       </c>
       <c r="I6">
-        <f>D6*100</f>
+        <f t="shared" si="3"/>
         <v>14.3250018358</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.107249997556</v>
       </c>
@@ -3543,23 +3571,23 @@
         <v>6</v>
       </c>
       <c r="F7">
-        <f>A7*100</f>
+        <f t="shared" si="0"/>
         <v>10.724999755599999</v>
       </c>
       <c r="G7">
-        <f>B7*100</f>
+        <f t="shared" si="1"/>
         <v>8.9250005781699997</v>
       </c>
       <c r="H7">
-        <f>C7*100</f>
+        <f t="shared" si="2"/>
         <v>10.399999469500001</v>
       </c>
       <c r="I7">
-        <f>D7*100</f>
+        <f t="shared" si="3"/>
         <v>12.0749995112</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.100499995053</v>
       </c>
@@ -3576,23 +3604,23 @@
         <v>7</v>
       </c>
       <c r="F8">
-        <f>A8*100</f>
+        <f t="shared" si="0"/>
         <v>10.049999505300001</v>
       </c>
       <c r="G8">
-        <f>B8*100</f>
+        <f t="shared" si="1"/>
         <v>7.87499919534</v>
       </c>
       <c r="H8">
-        <f>C8*100</f>
+        <f t="shared" si="2"/>
         <v>9.799999743699999</v>
       </c>
       <c r="I8">
-        <f>D8*100</f>
+        <f t="shared" si="3"/>
         <v>12.150000780799999</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8.9500010013600001E-2</v>
       </c>
@@ -3609,23 +3637,23 @@
         <v>8</v>
       </c>
       <c r="F9">
-        <f>A9*100</f>
+        <f t="shared" si="0"/>
         <v>8.9500010013600004</v>
       </c>
       <c r="G9">
-        <f>B9*100</f>
+        <f t="shared" si="1"/>
         <v>7.34999999404</v>
       </c>
       <c r="H9">
-        <f>C9*100</f>
+        <f t="shared" si="2"/>
         <v>9.7000002860999999</v>
       </c>
       <c r="I9">
-        <f>D9*100</f>
+        <f t="shared" si="3"/>
         <v>11.525000631800001</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8.2000009715599995E-2</v>
       </c>
@@ -3642,23 +3670,23 @@
         <v>9</v>
       </c>
       <c r="F10">
-        <f>A10*100</f>
+        <f t="shared" si="0"/>
         <v>8.2000009715599997</v>
       </c>
       <c r="G10">
-        <f>B10*100</f>
+        <f t="shared" si="1"/>
         <v>7.4500009417499999</v>
       </c>
       <c r="H10">
-        <f>C10*100</f>
+        <f t="shared" si="2"/>
         <v>9.8249994218300003</v>
       </c>
       <c r="I10">
-        <f>D10*100</f>
+        <f t="shared" si="3"/>
         <v>11.450000852300001</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7.3999993503100006E-2</v>
       </c>
@@ -3675,23 +3703,23 @@
         <v>10</v>
       </c>
       <c r="F11">
-        <f>A11*100</f>
+        <f t="shared" si="0"/>
         <v>7.3999993503100008</v>
       </c>
       <c r="G11">
-        <f>B11*100</f>
+        <f t="shared" si="1"/>
         <v>7.4500001967000005</v>
       </c>
       <c r="H11">
-        <f>C11*100</f>
+        <f t="shared" si="2"/>
         <v>9.6749991178499997</v>
       </c>
       <c r="I11">
-        <f>D11*100</f>
+        <f t="shared" si="3"/>
         <v>11.474998295300001</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>7.1249991655299993E-2</v>
       </c>
@@ -3708,23 +3736,23 @@
         <v>11</v>
       </c>
       <c r="F12">
-        <f>A12*100</f>
+        <f t="shared" si="0"/>
         <v>7.1249991655299993</v>
       </c>
       <c r="G12">
-        <f>B12*100</f>
+        <f t="shared" si="1"/>
         <v>7.2750009596299998</v>
       </c>
       <c r="H12">
-        <f>C12*100</f>
+        <f t="shared" si="2"/>
         <v>8.950000256300001</v>
       </c>
       <c r="I12">
-        <f>D12*100</f>
+        <f t="shared" si="3"/>
         <v>10.525000095399999</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6.8999990820899998E-2</v>
       </c>
@@ -3741,23 +3769,23 @@
         <v>12</v>
       </c>
       <c r="F13">
-        <f>A13*100</f>
+        <f t="shared" si="0"/>
         <v>6.8999990820899999</v>
       </c>
       <c r="G13">
-        <f>B13*100</f>
+        <f t="shared" si="1"/>
         <v>7.6499998569500001</v>
       </c>
       <c r="H13">
-        <f>C13*100</f>
+        <f t="shared" si="2"/>
         <v>8.6249992251399998</v>
       </c>
       <c r="I13">
-        <f>D13*100</f>
+        <f t="shared" si="3"/>
         <v>10.500000417200001</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6.3999995589300002E-2</v>
       </c>
@@ -3774,23 +3802,23 @@
         <v>13</v>
       </c>
       <c r="F14">
-        <f>A14*100</f>
+        <f t="shared" si="0"/>
         <v>6.3999995589300003</v>
       </c>
       <c r="G14">
-        <f>B14*100</f>
+        <f t="shared" si="1"/>
         <v>7.3749996721700004</v>
       </c>
       <c r="H14">
-        <f>C14*100</f>
+        <f t="shared" si="2"/>
         <v>8.3750002086199995</v>
       </c>
       <c r="I14">
-        <f>D14*100</f>
+        <f t="shared" si="3"/>
         <v>10.2999992669</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6.2499992549400002E-2</v>
       </c>
@@ -3807,23 +3835,23 @@
         <v>14</v>
       </c>
       <c r="F15">
-        <f>A15*100</f>
+        <f t="shared" si="0"/>
         <v>6.2499992549400005</v>
       </c>
       <c r="G15">
-        <f>B15*100</f>
+        <f t="shared" si="1"/>
         <v>7.3000013828299997</v>
       </c>
       <c r="H15">
-        <f>C15*100</f>
+        <f t="shared" si="2"/>
         <v>8.1500016152899999</v>
       </c>
       <c r="I15">
-        <f>D15*100</f>
+        <f t="shared" si="3"/>
         <v>10.149999707899999</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>6.1499994248199998E-2</v>
       </c>
@@ -3840,23 +3868,23 @@
         <v>15</v>
       </c>
       <c r="F16">
-        <f>A16*100</f>
+        <f t="shared" si="0"/>
         <v>6.1499994248199998</v>
       </c>
       <c r="G16">
-        <f>B16*100</f>
+        <f t="shared" si="1"/>
         <v>7.2999998927100007</v>
       </c>
       <c r="H16">
-        <f>C16*100</f>
+        <f t="shared" si="2"/>
         <v>7.75000080466</v>
       </c>
       <c r="I16">
-        <f>D16*100</f>
+        <f t="shared" si="3"/>
         <v>10.125000029800001</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>6.0749992728200003E-2</v>
       </c>
@@ -3873,23 +3901,23 @@
         <v>16</v>
       </c>
       <c r="F17">
-        <f>A17*100</f>
+        <f t="shared" si="0"/>
         <v>6.0749992728200004</v>
       </c>
       <c r="G17">
-        <f>B17*100</f>
+        <f t="shared" si="1"/>
         <v>7.2999998927100007</v>
       </c>
       <c r="H17">
-        <f>C17*100</f>
+        <f t="shared" si="2"/>
         <v>10.000000149</v>
       </c>
       <c r="I17">
-        <f>D17*100</f>
+        <f t="shared" si="3"/>
         <v>9.9750004708799995</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5.87499886751E-2</v>
       </c>
@@ -3906,23 +3934,23 @@
         <v>17</v>
       </c>
       <c r="F18">
-        <f>A18*100</f>
+        <f t="shared" si="0"/>
         <v>5.8749988675099996</v>
       </c>
       <c r="G18">
-        <f>B18*100</f>
+        <f t="shared" si="1"/>
         <v>7.34999999404</v>
       </c>
       <c r="H18">
-        <f>C18*100</f>
+        <f t="shared" si="2"/>
         <v>8.6000002920600007</v>
       </c>
       <c r="I18">
-        <f>D18*100</f>
+        <f t="shared" si="3"/>
         <v>9.8249994218300003</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5.8499988168500001E-2</v>
       </c>
@@ -3939,23 +3967,23 @@
         <v>18</v>
       </c>
       <c r="F19">
-        <f>A19*100</f>
+        <f t="shared" si="0"/>
         <v>5.8499988168500003</v>
       </c>
       <c r="G19">
-        <f>B19*100</f>
+        <f t="shared" si="1"/>
         <v>7.3999993503100008</v>
       </c>
       <c r="H19">
-        <f>C19*100</f>
+        <f t="shared" si="2"/>
         <v>8.2499995827700001</v>
       </c>
       <c r="I19">
-        <f>D19*100</f>
+        <f t="shared" si="3"/>
         <v>9.7249984741199995</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5.8999985456500002E-2</v>
       </c>
@@ -3972,23 +4000,23 @@
         <v>19</v>
       </c>
       <c r="F20">
-        <f>A20*100</f>
+        <f t="shared" si="0"/>
         <v>5.8999985456499999</v>
       </c>
       <c r="G20">
-        <f>B20*100</f>
+        <f t="shared" si="1"/>
         <v>7.4749991297700005</v>
       </c>
       <c r="H20">
-        <f>C20*100</f>
+        <f t="shared" si="2"/>
         <v>8.1249997019800002</v>
       </c>
       <c r="I20">
-        <f>D20*100</f>
+        <f t="shared" si="3"/>
         <v>9.6749983727900002</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>5.8499984443200002E-2</v>
       </c>
@@ -4005,23 +4033,23 @@
         <v>20</v>
       </c>
       <c r="F21">
-        <f>A21*100</f>
+        <f t="shared" si="0"/>
         <v>5.8499984443200006</v>
       </c>
       <c r="G21">
-        <f>B21*100</f>
+        <f t="shared" si="1"/>
         <v>7.4250005185600001</v>
       </c>
       <c r="H21">
-        <f>C21*100</f>
+        <f t="shared" si="2"/>
         <v>7.9999998211900003</v>
       </c>
       <c r="I21">
-        <f>D21*100</f>
+        <f t="shared" si="3"/>
         <v>9.6249990165200003</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>5.7499986141900002E-2</v>
       </c>
@@ -4038,23 +4066,23 @@
         <v>21</v>
       </c>
       <c r="F22">
-        <f>A22*100</f>
+        <f t="shared" si="0"/>
         <v>5.7499986141899999</v>
       </c>
       <c r="G22">
-        <f>B22*100</f>
+        <f t="shared" si="1"/>
         <v>7.4500001967000005</v>
       </c>
       <c r="H22">
-        <f>C22*100</f>
+        <f t="shared" si="2"/>
         <v>7.87499919534</v>
       </c>
       <c r="I22">
-        <f>D22*100</f>
+        <f t="shared" si="3"/>
         <v>9.499998390670001</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>5.6749988347300002E-2</v>
       </c>
@@ -4071,23 +4099,23 @@
         <v>22</v>
       </c>
       <c r="F23">
-        <f>A23*100</f>
+        <f t="shared" si="0"/>
         <v>5.6749988347300002</v>
       </c>
       <c r="G23">
-        <f>B23*100</f>
+        <f t="shared" si="1"/>
         <v>7.4500001967000005</v>
       </c>
       <c r="H23">
-        <f>C23*100</f>
+        <f t="shared" si="2"/>
         <v>7.8249998390700002</v>
       </c>
       <c r="I23">
-        <f>D23*100</f>
+        <f t="shared" si="3"/>
         <v>9.4749987125399997</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>5.64999915659E-2</v>
       </c>
@@ -4104,23 +4132,23 @@
         <v>23</v>
       </c>
       <c r="F24">
-        <f>A24*100</f>
+        <f t="shared" si="0"/>
         <v>5.6499991565899998</v>
       </c>
       <c r="G24">
-        <f>B24*100</f>
+        <f t="shared" si="1"/>
         <v>7.4000000953700003</v>
       </c>
       <c r="H24">
-        <f>C24*100</f>
+        <f t="shared" si="2"/>
         <v>7.8500010073199995</v>
       </c>
       <c r="I24">
-        <f>D24*100</f>
+        <f t="shared" si="3"/>
         <v>9.4750002026600004</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>5.6499995291199999E-2</v>
       </c>
@@ -4137,23 +4165,23 @@
         <v>24</v>
       </c>
       <c r="F25">
-        <f>A25*100</f>
+        <f t="shared" si="0"/>
         <v>5.6499995291199996</v>
       </c>
       <c r="G25">
-        <f>B25*100</f>
+        <f t="shared" si="1"/>
         <v>7.3250003159000006</v>
       </c>
       <c r="H25">
-        <f>C25*100</f>
+        <f t="shared" si="2"/>
         <v>7.77499973774</v>
       </c>
       <c r="I25">
-        <f>D25*100</f>
+        <f t="shared" si="3"/>
         <v>9.474999457600001</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>5.62499985099E-2</v>
       </c>
@@ -4170,23 +4198,23 @@
         <v>25</v>
       </c>
       <c r="F26">
-        <f>A26*100</f>
+        <f t="shared" si="0"/>
         <v>5.6249998509900001</v>
       </c>
       <c r="G26">
-        <f>B26*100</f>
+        <f t="shared" si="1"/>
         <v>7.2249993681899998</v>
       </c>
       <c r="H26">
-        <f>C26*100</f>
+        <f t="shared" si="2"/>
         <v>7.8000001609299998</v>
       </c>
       <c r="I26">
-        <f>D26*100</f>
+        <f t="shared" si="3"/>
         <v>9.4499990343999993</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>5.62499985099E-2</v>
       </c>
@@ -4203,23 +4231,23 @@
         <v>26</v>
       </c>
       <c r="F27">
-        <f>A27*100</f>
+        <f t="shared" si="0"/>
         <v>5.6249998509900001</v>
       </c>
       <c r="G27">
-        <f>B27*100</f>
+        <f t="shared" si="1"/>
         <v>7.1749992668599996</v>
       </c>
       <c r="H27">
-        <f>C27*100</f>
+        <f t="shared" si="2"/>
         <v>7.7999994158700003</v>
       </c>
       <c r="I27">
-        <f>D27*100</f>
+        <f t="shared" si="3"/>
         <v>9.375</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>5.6000001728499997E-2</v>
       </c>
@@ -4236,23 +4264,23 @@
         <v>27</v>
       </c>
       <c r="F28">
-        <f>A28*100</f>
+        <f t="shared" si="0"/>
         <v>5.6000001728499997</v>
       </c>
       <c r="G28">
-        <f>B28*100</f>
+        <f t="shared" si="1"/>
         <v>7.0999994873999999</v>
       </c>
       <c r="H28">
-        <f>C28*100</f>
+        <f t="shared" si="2"/>
         <v>7.7499993145500001</v>
       </c>
       <c r="I28">
-        <f>D28*100</f>
+        <f t="shared" si="3"/>
         <v>9.275000542399999</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>5.4999999702000001E-2</v>
       </c>
@@ -4269,23 +4297,23 @@
         <v>28</v>
       </c>
       <c r="F29">
-        <f>A29*100</f>
+        <f t="shared" si="0"/>
         <v>5.4999999702000002</v>
       </c>
       <c r="G29">
-        <f>B29*100</f>
+        <f t="shared" si="1"/>
         <v>7.0749998092699995</v>
       </c>
       <c r="H29">
-        <f>C29*100</f>
+        <f t="shared" si="2"/>
         <v>7.7499993145500001</v>
       </c>
       <c r="I29">
-        <f>D29*100</f>
+        <f t="shared" si="3"/>
         <v>9.3000002205399994</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>5.4249998182100002E-2</v>
       </c>
@@ -4302,23 +4330,23 @@
         <v>29</v>
       </c>
       <c r="F30">
-        <f>A30*100</f>
+        <f t="shared" si="0"/>
         <v>5.4249998182099999</v>
       </c>
       <c r="G30">
-        <f>B30*100</f>
+        <f t="shared" si="1"/>
         <v>7.0499993860699997</v>
       </c>
       <c r="H30">
-        <f>C30*100</f>
+        <f t="shared" si="2"/>
         <v>7.7249996364099998</v>
       </c>
       <c r="I30">
-        <f>D30*100</f>
+        <f t="shared" si="3"/>
         <v>9.275000542399999</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>5.4249998182100002E-2</v>
       </c>
@@ -4335,23 +4363,23 @@
         <v>30</v>
       </c>
       <c r="F31">
-        <f>A31*100</f>
+        <f t="shared" si="0"/>
         <v>5.4249998182099999</v>
       </c>
       <c r="G31">
-        <f>B31*100</f>
+        <f t="shared" si="1"/>
         <v>7.0499993860699997</v>
       </c>
       <c r="H31">
-        <f>C31*100</f>
+        <f t="shared" si="2"/>
         <v>7.6749995350800004</v>
       </c>
       <c r="I31">
-        <f>D31*100</f>
+        <f t="shared" si="3"/>
         <v>9.400000423189999</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>5.4249998182100002E-2</v>
       </c>
@@ -4368,23 +4396,23 @@
         <v>31</v>
       </c>
       <c r="F32">
-        <f>A32*100</f>
+        <f t="shared" si="0"/>
         <v>5.4249998182099999</v>
       </c>
       <c r="G32">
-        <f>B32*100</f>
+        <f t="shared" si="1"/>
         <v>7.0249989628799998</v>
       </c>
       <c r="H32">
-        <f>C32*100</f>
+        <f t="shared" si="2"/>
         <v>7.5749993324300009</v>
       </c>
       <c r="I32">
-        <f>D32*100</f>
+        <f t="shared" si="3"/>
         <v>9.4249993562699999</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>5.3999997675400001E-2</v>
       </c>
@@ -4401,23 +4429,23 @@
         <v>32</v>
       </c>
       <c r="F33">
-        <f>A33*100</f>
+        <f t="shared" si="0"/>
         <v>5.3999997675399998</v>
       </c>
       <c r="G33">
-        <f>B33*100</f>
+        <f t="shared" si="1"/>
         <v>6.97499960661</v>
       </c>
       <c r="H33">
-        <f>C33*100</f>
+        <f t="shared" si="2"/>
         <v>7.5749993324300009</v>
       </c>
       <c r="I33">
-        <f>D33*100</f>
+        <f t="shared" si="3"/>
         <v>9.4749987125399997</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>5.3999997675400001E-2</v>
       </c>
@@ -4434,23 +4462,23 @@
         <v>33</v>
       </c>
       <c r="F34">
-        <f>A34*100</f>
+        <f t="shared" ref="F34:F65" si="4">A34*100</f>
         <v>5.3999997675399998</v>
       </c>
       <c r="G34">
-        <f>B34*100</f>
+        <f t="shared" ref="G34:G65" si="5">B34*100</f>
         <v>6.9499999284700005</v>
       </c>
       <c r="H34">
-        <f>C34*100</f>
+        <f t="shared" ref="H34:H65" si="6">C34*100</f>
         <v>7.5249992311000007</v>
       </c>
       <c r="I34">
-        <f>D34*100</f>
+        <f t="shared" ref="I34:I65" si="7">D34*100</f>
         <v>9.4249993562699999</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>5.3749997168800003E-2</v>
       </c>
@@ -4467,23 +4495,23 @@
         <v>34</v>
       </c>
       <c r="F35">
-        <f>A35*100</f>
+        <f t="shared" si="4"/>
         <v>5.3749997168800006</v>
       </c>
       <c r="G35">
-        <f>B35*100</f>
+        <f t="shared" si="5"/>
         <v>6.8749994039499995</v>
       </c>
       <c r="H35">
-        <f>C35*100</f>
+        <f t="shared" si="6"/>
         <v>7.4749991297700005</v>
       </c>
       <c r="I35">
-        <f>D35*100</f>
+        <f t="shared" si="7"/>
         <v>9.4249993562699999</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>5.3499996662100001E-2</v>
       </c>
@@ -4500,23 +4528,23 @@
         <v>35</v>
       </c>
       <c r="F36">
-        <f>A36*100</f>
+        <f t="shared" si="4"/>
         <v>5.3499996662100004</v>
       </c>
       <c r="G36">
-        <f>B36*100</f>
+        <f t="shared" si="5"/>
         <v>6.8999998271499994</v>
       </c>
       <c r="H36">
-        <f>C36*100</f>
+        <f t="shared" si="6"/>
         <v>7.3999993503100008</v>
       </c>
       <c r="I36">
-        <f>D36*100</f>
+        <f t="shared" si="7"/>
         <v>9.274999052290001</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>5.3499996662100001E-2</v>
       </c>
@@ -4533,23 +4561,23 @@
         <v>36</v>
       </c>
       <c r="F37">
-        <f>A37*100</f>
+        <f t="shared" si="4"/>
         <v>5.3499996662100004</v>
       </c>
       <c r="G37">
-        <f>B37*100</f>
+        <f t="shared" si="5"/>
         <v>6.7999996244899998</v>
       </c>
       <c r="H37">
-        <f>C37*100</f>
+        <f t="shared" si="6"/>
         <v>7.3999993503100008</v>
       </c>
       <c r="I37">
-        <f>D37*100</f>
+        <f t="shared" si="7"/>
         <v>9.2499993741500006</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>5.3249996155500003E-2</v>
       </c>
@@ -4566,23 +4594,23 @@
         <v>37</v>
       </c>
       <c r="F38">
-        <f>A38*100</f>
+        <f t="shared" si="4"/>
         <v>5.3249996155500003</v>
       </c>
       <c r="G38">
-        <f>B38*100</f>
+        <f t="shared" si="5"/>
         <v>6.7999996244899998</v>
       </c>
       <c r="H38">
-        <f>C38*100</f>
+        <f t="shared" si="6"/>
         <v>7.4249997735000006</v>
       </c>
       <c r="I38">
-        <f>D38*100</f>
+        <f t="shared" si="7"/>
         <v>9.274999052290001</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>5.3749997168800003E-2</v>
       </c>
@@ -4599,23 +4627,23 @@
         <v>38</v>
       </c>
       <c r="F39">
-        <f>A39*100</f>
+        <f t="shared" si="4"/>
         <v>5.3749997168800006</v>
       </c>
       <c r="G39">
-        <f>B39*100</f>
+        <f t="shared" si="5"/>
         <v>6.7499995231599996</v>
       </c>
       <c r="H39">
-        <f>C39*100</f>
+        <f t="shared" si="6"/>
         <v>7.4749998748299999</v>
       </c>
       <c r="I39">
-        <f>D39*100</f>
+        <f t="shared" si="7"/>
         <v>9.2499986290900011</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>5.3749997168800003E-2</v>
       </c>
@@ -4632,23 +4660,23 @@
         <v>39</v>
       </c>
       <c r="F40">
-        <f>A40*100</f>
+        <f t="shared" si="4"/>
         <v>5.3749997168800006</v>
       </c>
       <c r="G40">
-        <f>B40*100</f>
+        <f t="shared" si="5"/>
         <v>6.7999996244899998</v>
       </c>
       <c r="H40">
-        <f>C40*100</f>
+        <f t="shared" si="6"/>
         <v>7.449999451640001</v>
       </c>
       <c r="I40">
-        <f>D40*100</f>
+        <f t="shared" si="7"/>
         <v>9.2249982058999986</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>5.3749997168800003E-2</v>
       </c>
@@ -4665,23 +4693,23 @@
         <v>40</v>
       </c>
       <c r="F41">
-        <f>A41*100</f>
+        <f t="shared" si="4"/>
         <v>5.3749997168800006</v>
       </c>
       <c r="G41">
-        <f>B41*100</f>
+        <f t="shared" si="5"/>
         <v>6.7499995231599996</v>
       </c>
       <c r="H41">
-        <f>C41*100</f>
+        <f t="shared" si="6"/>
         <v>7.3999993503100008</v>
       </c>
       <c r="I41">
-        <f>D41*100</f>
+        <f t="shared" si="7"/>
         <v>9.1999977827099997</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>5.3749997168800003E-2</v>
       </c>
@@ -4698,23 +4726,23 @@
         <v>41</v>
       </c>
       <c r="F42">
-        <f>A42*100</f>
+        <f t="shared" si="4"/>
         <v>5.3749997168800006</v>
       </c>
       <c r="G42">
-        <f>B42*100</f>
+        <f t="shared" si="5"/>
         <v>6.7249998450300001</v>
       </c>
       <c r="H42">
-        <f>C42*100</f>
+        <f t="shared" si="6"/>
         <v>7.3999993503100008</v>
       </c>
       <c r="I42">
-        <f>D42*100</f>
+        <f t="shared" si="7"/>
         <v>9.1499984264399998</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>5.3749997168800003E-2</v>
       </c>
@@ -4731,23 +4759,23 @@
         <v>42</v>
       </c>
       <c r="F43">
-        <f>A43*100</f>
+        <f t="shared" si="4"/>
         <v>5.3749997168800006</v>
       </c>
       <c r="G43">
-        <f>B43*100</f>
+        <f t="shared" si="5"/>
         <v>6.6999994218299994</v>
       </c>
       <c r="H43">
-        <f>C43*100</f>
+        <f t="shared" si="6"/>
         <v>7.3749996721700004</v>
       </c>
       <c r="I43">
-        <f>D43*100</f>
+        <f t="shared" si="7"/>
         <v>9.1499991715000011</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>5.3499996662100001E-2</v>
       </c>
@@ -4764,23 +4792,23 @@
         <v>43</v>
       </c>
       <c r="F44">
-        <f>A44*100</f>
+        <f t="shared" si="4"/>
         <v>5.3499996662100004</v>
       </c>
       <c r="G44">
-        <f>B44*100</f>
+        <f t="shared" si="5"/>
         <v>6.6499993205100001</v>
       </c>
       <c r="H44">
-        <f>C44*100</f>
+        <f t="shared" si="6"/>
         <v>7.3749996721700004</v>
       </c>
       <c r="I44">
-        <f>D44*100</f>
+        <f t="shared" si="7"/>
         <v>9.1499991715000011</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>5.3499996662100001E-2</v>
       </c>
@@ -4797,23 +4825,23 @@
         <v>44</v>
       </c>
       <c r="F45">
-        <f>A45*100</f>
+        <f t="shared" si="4"/>
         <v>5.3499996662100004</v>
       </c>
       <c r="G45">
-        <f>B45*100</f>
+        <f t="shared" si="5"/>
         <v>6.6249996423699997</v>
       </c>
       <c r="H45">
-        <f>C45*100</f>
+        <f t="shared" si="6"/>
         <v>7.3499992489800006</v>
       </c>
       <c r="I45">
-        <f>D45*100</f>
+        <f t="shared" si="7"/>
         <v>9.1249994933600007</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>5.3499996662100001E-2</v>
       </c>
@@ -4830,23 +4858,23 @@
         <v>45</v>
       </c>
       <c r="F46">
-        <f>A46*100</f>
+        <f t="shared" si="4"/>
         <v>5.3499996662100004</v>
       </c>
       <c r="G46">
-        <f>B46*100</f>
+        <f t="shared" si="5"/>
         <v>6.6499993205100001</v>
       </c>
       <c r="H46">
-        <f>C46*100</f>
+        <f t="shared" si="6"/>
         <v>7.3499992489800006</v>
       </c>
       <c r="I46">
-        <f>D46*100</f>
+        <f t="shared" si="7"/>
         <v>9.0999998152300012</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>5.3749997168800003E-2</v>
       </c>
@@ -4863,23 +4891,23 @@
         <v>46</v>
       </c>
       <c r="F47">
-        <f>A47*100</f>
+        <f t="shared" si="4"/>
         <v>5.3749997168800006</v>
       </c>
       <c r="G47">
-        <f>B47*100</f>
+        <f t="shared" si="5"/>
         <v>6.3749998807899999</v>
       </c>
       <c r="H47">
-        <f>C47*100</f>
+        <f t="shared" si="6"/>
         <v>7.3499992489800006</v>
       </c>
       <c r="I47">
-        <f>D47*100</f>
+        <f t="shared" si="7"/>
         <v>9.1250002384200002</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>5.3749997168800003E-2</v>
       </c>
@@ -4896,23 +4924,23 @@
         <v>47</v>
       </c>
       <c r="F48">
-        <f>A48*100</f>
+        <f t="shared" si="4"/>
         <v>5.3749997168800006</v>
       </c>
       <c r="G48">
-        <f>B48*100</f>
+        <f t="shared" si="5"/>
         <v>6.4000003039799997</v>
       </c>
       <c r="H48">
-        <f>C48*100</f>
+        <f t="shared" si="6"/>
         <v>7.3249995708499993</v>
       </c>
       <c r="I48">
-        <f>D48*100</f>
+        <f t="shared" si="7"/>
         <v>9.0750001370900009</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>5.3999997675400001E-2</v>
       </c>
@@ -4929,23 +4957,23 @@
         <v>48</v>
       </c>
       <c r="F49">
-        <f>A49*100</f>
+        <f t="shared" si="4"/>
         <v>5.3999997675399998</v>
       </c>
       <c r="G49">
-        <f>B49*100</f>
+        <f t="shared" si="5"/>
         <v>6.4249999821200001</v>
       </c>
       <c r="H49">
-        <f>C49*100</f>
+        <f t="shared" si="6"/>
         <v>7.3499992489800006</v>
       </c>
       <c r="I49">
-        <f>D49*100</f>
+        <f t="shared" si="7"/>
         <v>9.0750001370900009</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>5.4249998182100002E-2</v>
       </c>
@@ -4962,23 +4990,23 @@
         <v>49</v>
       </c>
       <c r="F50">
-        <f>A50*100</f>
+        <f t="shared" si="4"/>
         <v>5.4249998182099999</v>
       </c>
       <c r="G50">
-        <f>B50*100</f>
+        <f t="shared" si="5"/>
         <v>6.4249999821200001</v>
       </c>
       <c r="H50">
-        <f>C50*100</f>
+        <f t="shared" si="6"/>
         <v>7.3499992489800006</v>
       </c>
       <c r="I50">
-        <f>D50*100</f>
+        <f t="shared" si="7"/>
         <v>9.0750001370900009</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>5.4250001907299998E-2</v>
       </c>
@@ -4995,23 +5023,23 @@
         <v>50</v>
       </c>
       <c r="F51">
-        <f>A51*100</f>
+        <f t="shared" si="4"/>
         <v>5.4250001907299996</v>
       </c>
       <c r="G51">
-        <f>B51*100</f>
+        <f t="shared" si="5"/>
         <v>6.4249999821200001</v>
       </c>
       <c r="H51">
-        <f>C51*100</f>
+        <f t="shared" si="6"/>
         <v>7.3249995708499993</v>
       </c>
       <c r="I51">
-        <f>D51*100</f>
+        <f t="shared" si="7"/>
         <v>9.0500004589599996</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>5.4250001907299998E-2</v>
       </c>
@@ -5028,23 +5056,23 @@
         <v>51</v>
       </c>
       <c r="F52">
-        <f>A52*100</f>
+        <f t="shared" si="4"/>
         <v>5.4250001907299996</v>
       </c>
       <c r="G52">
-        <f>B52*100</f>
+        <f t="shared" si="5"/>
         <v>6.45000040531</v>
       </c>
       <c r="H52">
-        <f>C52*100</f>
+        <f t="shared" si="6"/>
         <v>7.3499992489800006</v>
       </c>
       <c r="I52">
-        <f>D52*100</f>
+        <f t="shared" si="7"/>
         <v>9.0750001370900009</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>5.4250001907299998E-2</v>
       </c>
@@ -5061,23 +5089,23 @@
         <v>52</v>
       </c>
       <c r="F53">
-        <f>A53*100</f>
+        <f t="shared" si="4"/>
         <v>5.4250001907299996</v>
       </c>
       <c r="G53">
-        <f>B53*100</f>
+        <f t="shared" si="5"/>
         <v>6.4000003039799997</v>
       </c>
       <c r="H53">
-        <f>C53*100</f>
+        <f t="shared" si="6"/>
         <v>7.3499992489800006</v>
       </c>
       <c r="I53">
-        <f>D53*100</f>
+        <f t="shared" si="7"/>
         <v>9.1249994933600007</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>5.3999997675400001E-2</v>
       </c>
@@ -5094,23 +5122,23 @@
         <v>53</v>
       </c>
       <c r="F54">
-        <f>A54*100</f>
+        <f t="shared" si="4"/>
         <v>5.3999997675399998</v>
       </c>
       <c r="G54">
-        <f>B54*100</f>
+        <f t="shared" si="5"/>
         <v>6.3749998807899999</v>
       </c>
       <c r="H54">
-        <f>C54*100</f>
+        <f t="shared" si="6"/>
         <v>7.3249995708499993</v>
       </c>
       <c r="I54">
-        <f>D54*100</f>
+        <f t="shared" si="7"/>
         <v>9.1249994933600007</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>5.3999997675400001E-2</v>
       </c>
@@ -5127,23 +5155,23 @@
         <v>54</v>
       </c>
       <c r="F55">
-        <f>A55*100</f>
+        <f t="shared" si="4"/>
         <v>5.3999997675399998</v>
       </c>
       <c r="G55">
-        <f>B55*100</f>
+        <f t="shared" si="5"/>
         <v>6.3500002026600004</v>
       </c>
       <c r="H55">
-        <f>C55*100</f>
+        <f t="shared" si="6"/>
         <v>7.34999999404</v>
       </c>
       <c r="I55">
-        <f>D55*100</f>
+        <f t="shared" si="7"/>
         <v>9.1249994933600007</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>5.3999997675400001E-2</v>
       </c>
@@ -5160,23 +5188,23 @@
         <v>55</v>
       </c>
       <c r="F56">
-        <f>A56*100</f>
+        <f t="shared" si="4"/>
         <v>5.3999997675399998</v>
       </c>
       <c r="G56">
-        <f>B56*100</f>
+        <f t="shared" si="5"/>
         <v>6.3000001013300002</v>
       </c>
       <c r="H56">
-        <f>C56*100</f>
+        <f t="shared" si="6"/>
         <v>7.34999999404</v>
       </c>
       <c r="I56">
-        <f>D56*100</f>
+        <f t="shared" si="7"/>
         <v>9.1249994933600007</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>5.3999997675400001E-2</v>
       </c>
@@ -5193,23 +5221,23 @@
         <v>56</v>
       </c>
       <c r="F57">
-        <f>A57*100</f>
+        <f t="shared" si="4"/>
         <v>5.3999997675399998</v>
       </c>
       <c r="G57">
-        <f>B57*100</f>
+        <f t="shared" si="5"/>
         <v>6.25</v>
       </c>
       <c r="H57">
-        <f>C57*100</f>
+        <f t="shared" si="6"/>
         <v>7.34999999404</v>
       </c>
       <c r="I57">
-        <f>D57*100</f>
+        <f t="shared" si="7"/>
         <v>9.1499991715000011</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>5.4249998182100002E-2</v>
       </c>
@@ -5226,23 +5254,23 @@
         <v>57</v>
       </c>
       <c r="F58">
-        <f>A58*100</f>
+        <f t="shared" si="4"/>
         <v>5.4249998182099999</v>
       </c>
       <c r="G58">
-        <f>B58*100</f>
+        <f t="shared" si="5"/>
         <v>6.3000001013300002</v>
       </c>
       <c r="H58">
-        <f>C58*100</f>
+        <f t="shared" si="6"/>
         <v>7.2999991476500004</v>
       </c>
       <c r="I58">
-        <f>D58*100</f>
+        <f t="shared" si="7"/>
         <v>9.1750003397499995</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>5.4249998182100002E-2</v>
       </c>
@@ -5259,23 +5287,23 @@
         <v>58</v>
       </c>
       <c r="F59">
-        <f>A59*100</f>
+        <f t="shared" si="4"/>
         <v>5.4249998182099999</v>
       </c>
       <c r="G59">
-        <f>B59*100</f>
+        <f t="shared" si="5"/>
         <v>6.2750004231899998</v>
       </c>
       <c r="H59">
-        <f>C59*100</f>
+        <f t="shared" si="6"/>
         <v>7.2999991476500004</v>
       </c>
       <c r="I59">
-        <f>D59*100</f>
+        <f t="shared" si="7"/>
         <v>9.2249996960200011</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>5.4249998182100002E-2</v>
       </c>
@@ -5292,23 +5320,23 @@
         <v>59</v>
       </c>
       <c r="F60">
-        <f>A60*100</f>
+        <f t="shared" si="4"/>
         <v>5.4249998182099999</v>
       </c>
       <c r="G60">
-        <f>B60*100</f>
+        <f t="shared" si="5"/>
         <v>6.2750004231899998</v>
       </c>
       <c r="H60">
-        <f>C60*100</f>
+        <f t="shared" si="6"/>
         <v>7.3249995708499993</v>
       </c>
       <c r="I60">
-        <f>D60*100</f>
+        <f t="shared" si="7"/>
         <v>9.2249996960200011</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>5.4249998182100002E-2</v>
       </c>
@@ -5325,23 +5353,23 @@
         <v>60</v>
       </c>
       <c r="F61">
-        <f>A61*100</f>
+        <f t="shared" si="4"/>
         <v>5.4249998182099999</v>
       </c>
       <c r="G61">
-        <f>B61*100</f>
+        <f t="shared" si="5"/>
         <v>6.2750004231899998</v>
       </c>
       <c r="H61">
-        <f>C61*100</f>
+        <f t="shared" si="6"/>
         <v>7.3249995708499993</v>
       </c>
       <c r="I61">
-        <f>D61*100</f>
+        <f t="shared" si="7"/>
         <v>9.274999052290001</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>5.4249998182100002E-2</v>
       </c>
@@ -5358,23 +5386,23 @@
         <v>61</v>
       </c>
       <c r="F62">
-        <f>A62*100</f>
+        <f t="shared" si="4"/>
         <v>5.4249998182099999</v>
       </c>
       <c r="G62">
-        <f>B62*100</f>
+        <f t="shared" si="5"/>
         <v>6.2750004231899998</v>
       </c>
       <c r="H62">
-        <f>C62*100</f>
+        <f t="shared" si="6"/>
         <v>7.3249995708499993</v>
       </c>
       <c r="I62">
-        <f>D62*100</f>
+        <f t="shared" si="7"/>
         <v>9.275000542399999</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>5.3999997675400001E-2</v>
       </c>
@@ -5391,23 +5419,23 @@
         <v>62</v>
       </c>
       <c r="F63">
-        <f>A63*100</f>
+        <f t="shared" si="4"/>
         <v>5.3999997675399998</v>
       </c>
       <c r="G63">
-        <f>B63*100</f>
+        <f t="shared" si="5"/>
         <v>6.3250005245200001</v>
       </c>
       <c r="H63">
-        <f>C63*100</f>
+        <f t="shared" si="6"/>
         <v>7.3249995708499993</v>
       </c>
       <c r="I63">
-        <f>D63*100</f>
+        <f t="shared" si="7"/>
         <v>9.2249996960200011</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>5.3999997675400001E-2</v>
       </c>
@@ -5424,23 +5452,23 @@
         <v>63</v>
       </c>
       <c r="F64">
-        <f>A64*100</f>
+        <f t="shared" si="4"/>
         <v>5.3999997675399998</v>
       </c>
       <c r="G64">
-        <f>B64*100</f>
+        <f t="shared" si="5"/>
         <v>6.3250005245200001</v>
       </c>
       <c r="H64">
-        <f>C64*100</f>
+        <f t="shared" si="6"/>
         <v>7.3499992489800006</v>
       </c>
       <c r="I64">
-        <f>D64*100</f>
+        <f t="shared" si="7"/>
         <v>9.2249996960200011</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>5.3999997675400001E-2</v>
       </c>
@@ -5457,23 +5485,23 @@
         <v>64</v>
       </c>
       <c r="F65">
-        <f>A65*100</f>
+        <f t="shared" si="4"/>
         <v>5.3999997675399998</v>
       </c>
       <c r="G65">
-        <f>B65*100</f>
+        <f t="shared" si="5"/>
         <v>6.350000947709999</v>
       </c>
       <c r="H65">
-        <f>C65*100</f>
+        <f t="shared" si="6"/>
         <v>7.3499992489800006</v>
       </c>
       <c r="I65">
-        <f>D65*100</f>
+        <f t="shared" si="7"/>
         <v>9.2249996960200011</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>5.3999997675400001E-2</v>
       </c>
@@ -5490,23 +5518,23 @@
         <v>65</v>
       </c>
       <c r="F66">
-        <f>A66*100</f>
+        <f t="shared" ref="F66:F102" si="8">A66*100</f>
         <v>5.3999997675399998</v>
       </c>
       <c r="G66">
-        <f>B66*100</f>
+        <f t="shared" ref="G66:G102" si="9">B66*100</f>
         <v>6.3250005245200001</v>
       </c>
       <c r="H66">
-        <f>C66*100</f>
+        <f t="shared" ref="H66:H102" si="10">C66*100</f>
         <v>7.3249995708499993</v>
       </c>
       <c r="I66">
-        <f>D66*100</f>
+        <f t="shared" ref="I66:I102" si="11">D66*100</f>
         <v>9.1750003397499995</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>5.3999997675400001E-2</v>
       </c>
@@ -5523,23 +5551,23 @@
         <v>66</v>
       </c>
       <c r="F67">
-        <f>A67*100</f>
+        <f t="shared" si="8"/>
         <v>5.3999997675399998</v>
       </c>
       <c r="G67">
-        <f>B67*100</f>
+        <f t="shared" si="9"/>
         <v>6.3250005245200001</v>
       </c>
       <c r="H67">
-        <f>C67*100</f>
+        <f t="shared" si="10"/>
         <v>7.2749994695199991</v>
       </c>
       <c r="I67">
-        <f>D67*100</f>
+        <f t="shared" si="11"/>
         <v>9.1750003397499995</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>5.4249998182100002E-2</v>
       </c>
@@ -5556,23 +5584,23 @@
         <v>67</v>
       </c>
       <c r="F68">
-        <f>A68*100</f>
+        <f t="shared" si="8"/>
         <v>5.4249998182099999</v>
       </c>
       <c r="G68">
-        <f>B68*100</f>
+        <f t="shared" si="9"/>
         <v>6.2750004231899998</v>
       </c>
       <c r="H68">
-        <f>C68*100</f>
+        <f t="shared" si="10"/>
         <v>7.2749994695199991</v>
       </c>
       <c r="I68">
-        <f>D68*100</f>
+        <f t="shared" si="11"/>
         <v>9.1499991715000011</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>5.3999997675400001E-2</v>
       </c>
@@ -5589,23 +5617,23 @@
         <v>68</v>
       </c>
       <c r="F69">
-        <f>A69*100</f>
+        <f t="shared" si="8"/>
         <v>5.3999997675399998</v>
       </c>
       <c r="G69">
-        <f>B69*100</f>
+        <f t="shared" si="9"/>
         <v>6.2750004231899998</v>
       </c>
       <c r="H69">
-        <f>C69*100</f>
+        <f t="shared" si="10"/>
         <v>7.2749994695199991</v>
       </c>
       <c r="I69">
-        <f>D69*100</f>
+        <f t="shared" si="11"/>
         <v>9.1499991715000011</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>5.3999997675400001E-2</v>
       </c>
@@ -5622,23 +5650,23 @@
         <v>69</v>
       </c>
       <c r="F70">
-        <f>A70*100</f>
+        <f t="shared" si="8"/>
         <v>5.3999997675399998</v>
       </c>
       <c r="G70">
-        <f>B70*100</f>
+        <f t="shared" si="9"/>
         <v>6.2750004231899998</v>
       </c>
       <c r="H70">
-        <f>C70*100</f>
+        <f t="shared" si="10"/>
         <v>7.2749994695199991</v>
       </c>
       <c r="I70">
-        <f>D70*100</f>
+        <f t="shared" si="11"/>
         <v>9.1249994933600007</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>5.3499996662100001E-2</v>
       </c>
@@ -5655,23 +5683,23 @@
         <v>70</v>
       </c>
       <c r="F71">
-        <f>A71*100</f>
+        <f t="shared" si="8"/>
         <v>5.3499996662100004</v>
       </c>
       <c r="G71">
-        <f>B71*100</f>
+        <f t="shared" si="9"/>
         <v>6.2750004231899998</v>
       </c>
       <c r="H71">
-        <f>C71*100</f>
+        <f t="shared" si="10"/>
         <v>7.2749994695199991</v>
       </c>
       <c r="I71">
-        <f>D71*100</f>
+        <f t="shared" si="11"/>
         <v>9.1249994933600007</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>5.3499996662100001E-2</v>
       </c>
@@ -5688,23 +5716,23 @@
         <v>71</v>
       </c>
       <c r="F72">
-        <f>A72*100</f>
+        <f t="shared" si="8"/>
         <v>5.3499996662100004</v>
       </c>
       <c r="G72">
-        <f>B72*100</f>
+        <f t="shared" si="9"/>
         <v>6.2750004231899998</v>
       </c>
       <c r="H72">
-        <f>C72*100</f>
+        <f t="shared" si="10"/>
         <v>7.3249995708499993</v>
       </c>
       <c r="I72">
-        <f>D72*100</f>
+        <f t="shared" si="11"/>
         <v>9.1500006616099991</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>5.3499996662100001E-2</v>
       </c>
@@ -5721,23 +5749,23 @@
         <v>72</v>
       </c>
       <c r="F73">
-        <f>A73*100</f>
+        <f t="shared" si="8"/>
         <v>5.3499996662100004</v>
       </c>
       <c r="G73">
-        <f>B73*100</f>
+        <f t="shared" si="9"/>
         <v>6.2750004231899998</v>
       </c>
       <c r="H73">
-        <f>C73*100</f>
+        <f t="shared" si="10"/>
         <v>7.3249995708499993</v>
       </c>
       <c r="I73">
-        <f>D73*100</f>
+        <f t="shared" si="11"/>
         <v>9.1750003397499995</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>5.3499996662100001E-2</v>
       </c>
@@ -5754,23 +5782,23 @@
         <v>73</v>
       </c>
       <c r="F74">
-        <f>A74*100</f>
+        <f t="shared" si="8"/>
         <v>5.3499996662100004</v>
       </c>
       <c r="G74">
-        <f>B74*100</f>
+        <f t="shared" si="9"/>
         <v>6.2750004231899998</v>
       </c>
       <c r="H74">
-        <f>C74*100</f>
+        <f t="shared" si="10"/>
         <v>7.3249995708499993</v>
       </c>
       <c r="I74">
-        <f>D74*100</f>
+        <f t="shared" si="11"/>
         <v>9.1750003397499995</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>5.2999995648899997E-2</v>
       </c>
@@ -5787,23 +5815,23 @@
         <v>74</v>
       </c>
       <c r="F75">
-        <f>A75*100</f>
+        <f t="shared" si="8"/>
         <v>5.2999995648899993</v>
       </c>
       <c r="G75">
-        <f>B75*100</f>
+        <f t="shared" si="9"/>
         <v>6.2750004231899998</v>
       </c>
       <c r="H75">
-        <f>C75*100</f>
+        <f t="shared" si="10"/>
         <v>7.3499992489800006</v>
       </c>
       <c r="I75">
-        <f>D75*100</f>
+        <f t="shared" si="11"/>
         <v>9.1500006616099991</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>5.2999995648899997E-2</v>
       </c>
@@ -5820,23 +5848,23 @@
         <v>75</v>
       </c>
       <c r="F76">
-        <f>A76*100</f>
+        <f t="shared" si="8"/>
         <v>5.2999995648899993</v>
       </c>
       <c r="G76">
-        <f>B76*100</f>
+        <f t="shared" si="9"/>
         <v>6.2750004231899998</v>
       </c>
       <c r="H76">
-        <f>C76*100</f>
+        <f t="shared" si="10"/>
         <v>7.3499992489800006</v>
       </c>
       <c r="I76">
-        <f>D76*100</f>
+        <f t="shared" si="11"/>
         <v>9.1500006616099991</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>5.3249999880800002E-2</v>
       </c>
@@ -5853,23 +5881,23 @@
         <v>76</v>
       </c>
       <c r="F77">
-        <f>A77*100</f>
+        <f t="shared" si="8"/>
         <v>5.3249999880800001</v>
       </c>
       <c r="G77">
-        <f>B77*100</f>
+        <f t="shared" si="9"/>
         <v>6.3000008463899997</v>
       </c>
       <c r="H77">
-        <f>C77*100</f>
+        <f t="shared" si="10"/>
         <v>7.3249995708499993</v>
       </c>
       <c r="I77">
-        <f>D77*100</f>
+        <f t="shared" si="11"/>
         <v>9.1500006616099991</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>5.2999999374200003E-2</v>
       </c>
@@ -5886,23 +5914,23 @@
         <v>77</v>
       </c>
       <c r="F78">
-        <f>A78*100</f>
+        <f t="shared" si="8"/>
         <v>5.29999993742</v>
       </c>
       <c r="G78">
-        <f>B78*100</f>
+        <f t="shared" si="9"/>
         <v>6.3000008463899997</v>
       </c>
       <c r="H78">
-        <f>C78*100</f>
+        <f t="shared" si="10"/>
         <v>7.3249995708499993</v>
       </c>
       <c r="I78">
-        <f>D78*100</f>
+        <f t="shared" si="11"/>
         <v>9.1500006616099991</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>5.3249999880800002E-2</v>
       </c>
@@ -5919,23 +5947,23 @@
         <v>78</v>
       </c>
       <c r="F79">
-        <f>A79*100</f>
+        <f t="shared" si="8"/>
         <v>5.3249999880800001</v>
       </c>
       <c r="G79">
-        <f>B79*100</f>
+        <f t="shared" si="9"/>
         <v>6.3000008463899997</v>
       </c>
       <c r="H79">
-        <f>C79*100</f>
+        <f t="shared" si="10"/>
         <v>7.3249995708499993</v>
       </c>
       <c r="I79">
-        <f>D79*100</f>
+        <f t="shared" si="11"/>
         <v>9.1500006616099991</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>5.3249996155500003E-2</v>
       </c>
@@ -5952,23 +5980,23 @@
         <v>79</v>
       </c>
       <c r="F80">
-        <f>A80*100</f>
+        <f t="shared" si="8"/>
         <v>5.3249996155500003</v>
       </c>
       <c r="G80">
-        <f>B80*100</f>
+        <f t="shared" si="9"/>
         <v>6.3000008463899997</v>
       </c>
       <c r="H80">
-        <f>C80*100</f>
+        <f t="shared" si="10"/>
         <v>7.3249995708499993</v>
       </c>
       <c r="I80">
-        <f>D80*100</f>
+        <f t="shared" si="11"/>
         <v>9.1500006616099991</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>5.2999995648899997E-2</v>
       </c>
@@ -5985,23 +6013,23 @@
         <v>80</v>
       </c>
       <c r="F81">
-        <f>A81*100</f>
+        <f t="shared" si="8"/>
         <v>5.2999995648899993</v>
       </c>
       <c r="G81">
-        <f>B81*100</f>
+        <f t="shared" si="9"/>
         <v>6.3000008463899997</v>
       </c>
       <c r="H81">
-        <f>C81*100</f>
+        <f t="shared" si="10"/>
         <v>7.3249995708499993</v>
       </c>
       <c r="I81">
-        <f>D81*100</f>
+        <f t="shared" si="11"/>
         <v>9.1750003397499995</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>5.2999995648899997E-2</v>
       </c>
@@ -6018,23 +6046,23 @@
         <v>81</v>
       </c>
       <c r="F82">
-        <f>A82*100</f>
+        <f t="shared" si="8"/>
         <v>5.2999995648899993</v>
       </c>
       <c r="G82">
-        <f>B82*100</f>
+        <f t="shared" si="9"/>
         <v>6.3000008463899997</v>
       </c>
       <c r="H82">
-        <f>C82*100</f>
+        <f t="shared" si="10"/>
         <v>7.3249995708499993</v>
       </c>
       <c r="I82">
-        <f>D82*100</f>
+        <f t="shared" si="11"/>
         <v>9.1499991715000011</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>5.2999995648899997E-2</v>
       </c>
@@ -6051,23 +6079,23 @@
         <v>82</v>
       </c>
       <c r="F83">
-        <f>A83*100</f>
+        <f t="shared" si="8"/>
         <v>5.2999995648899993</v>
       </c>
       <c r="G83">
-        <f>B83*100</f>
+        <f t="shared" si="9"/>
         <v>6.3000008463899997</v>
       </c>
       <c r="H83">
-        <f>C83*100</f>
+        <f t="shared" si="10"/>
         <v>7.3249995708499993</v>
       </c>
       <c r="I83">
-        <f>D83*100</f>
+        <f t="shared" si="11"/>
         <v>9.1249994933600007</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>5.2749995142200003E-2</v>
       </c>
@@ -6084,23 +6112,23 @@
         <v>83</v>
       </c>
       <c r="F84">
-        <f>A84*100</f>
+        <f t="shared" si="8"/>
         <v>5.2749995142200001</v>
       </c>
       <c r="G84">
-        <f>B84*100</f>
+        <f t="shared" si="9"/>
         <v>6.3000008463899997</v>
       </c>
       <c r="H84">
-        <f>C84*100</f>
+        <f t="shared" si="10"/>
         <v>7.3249995708499993</v>
       </c>
       <c r="I84">
-        <f>D84*100</f>
+        <f t="shared" si="11"/>
         <v>9.1500006616099991</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>5.2749995142200003E-2</v>
       </c>
@@ -6117,23 +6145,23 @@
         <v>84</v>
       </c>
       <c r="F85">
-        <f>A85*100</f>
+        <f t="shared" si="8"/>
         <v>5.2749995142200001</v>
       </c>
       <c r="G85">
-        <f>B85*100</f>
+        <f t="shared" si="9"/>
         <v>6.2750004231899998</v>
       </c>
       <c r="H85">
-        <f>C85*100</f>
+        <f t="shared" si="10"/>
         <v>7.34999999404</v>
       </c>
       <c r="I85">
-        <f>D85*100</f>
+        <f t="shared" si="11"/>
         <v>9.1249994933600007</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>5.2749995142200003E-2</v>
       </c>
@@ -6150,23 +6178,23 @@
         <v>85</v>
       </c>
       <c r="F86">
-        <f>A86*100</f>
+        <f t="shared" si="8"/>
         <v>5.2749995142200001</v>
       </c>
       <c r="G86">
-        <f>B86*100</f>
+        <f t="shared" si="9"/>
         <v>6.3000001013300002</v>
       </c>
       <c r="H86">
-        <f>C86*100</f>
+        <f t="shared" si="10"/>
         <v>7.34999999404</v>
       </c>
       <c r="I86">
-        <f>D86*100</f>
+        <f t="shared" si="11"/>
         <v>9.0999998152300012</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>5.3249996155500003E-2</v>
       </c>
@@ -6183,23 +6211,23 @@
         <v>86</v>
       </c>
       <c r="F87">
-        <f>A87*100</f>
+        <f t="shared" si="8"/>
         <v>5.3249996155500003</v>
       </c>
       <c r="G87">
-        <f>B87*100</f>
+        <f t="shared" si="9"/>
         <v>6.3000001013300002</v>
       </c>
       <c r="H87">
-        <f>C87*100</f>
+        <f t="shared" si="10"/>
         <v>7.4000000953700003</v>
       </c>
       <c r="I87">
-        <f>D87*100</f>
+        <f t="shared" si="11"/>
         <v>9.0750001370900009</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>5.3249996155500003E-2</v>
       </c>
@@ -6216,23 +6244,23 @@
         <v>87</v>
       </c>
       <c r="F88">
-        <f>A88*100</f>
+        <f t="shared" si="8"/>
         <v>5.3249996155500003</v>
       </c>
       <c r="G88">
-        <f>B88*100</f>
+        <f t="shared" si="9"/>
         <v>6.3000001013300002</v>
       </c>
       <c r="H88">
-        <f>C88*100</f>
+        <f t="shared" si="10"/>
         <v>7.3749996721700004</v>
       </c>
       <c r="I88">
-        <f>D88*100</f>
+        <f t="shared" si="11"/>
         <v>9.0750001370900009</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>5.3249996155500003E-2</v>
       </c>
@@ -6249,23 +6277,23 @@
         <v>88</v>
       </c>
       <c r="F89">
-        <f>A89*100</f>
+        <f t="shared" si="8"/>
         <v>5.3249996155500003</v>
       </c>
       <c r="G89">
-        <f>B89*100</f>
+        <f t="shared" si="9"/>
         <v>6.3250005245200001</v>
       </c>
       <c r="H89">
-        <f>C89*100</f>
+        <f t="shared" si="10"/>
         <v>7.3749996721700004</v>
       </c>
       <c r="I89">
-        <f>D89*100</f>
+        <f t="shared" si="11"/>
         <v>9.0750001370900009</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>5.2749995142200003E-2</v>
       </c>
@@ -6282,23 +6310,23 @@
         <v>89</v>
       </c>
       <c r="F90">
-        <f>A90*100</f>
+        <f t="shared" si="8"/>
         <v>5.2749995142200001</v>
       </c>
       <c r="G90">
-        <f>B90*100</f>
+        <f t="shared" si="9"/>
         <v>6.3250005245200001</v>
       </c>
       <c r="H90">
-        <f>C90*100</f>
+        <f t="shared" si="10"/>
         <v>7.3749996721700004</v>
       </c>
       <c r="I90">
-        <f>D90*100</f>
+        <f t="shared" si="11"/>
         <v>9.1499991715000011</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>5.2749995142200003E-2</v>
       </c>
@@ -6315,23 +6343,23 @@
         <v>90</v>
       </c>
       <c r="F91">
-        <f>A91*100</f>
+        <f t="shared" si="8"/>
         <v>5.2749995142200001</v>
       </c>
       <c r="G91">
-        <f>B91*100</f>
+        <f t="shared" si="9"/>
         <v>6.3250005245200001</v>
       </c>
       <c r="H91">
-        <f>C91*100</f>
+        <f t="shared" si="10"/>
         <v>7.3749996721700004</v>
       </c>
       <c r="I91">
-        <f>D91*100</f>
+        <f t="shared" si="11"/>
         <v>9.1499991715000011</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>5.2749995142200003E-2</v>
       </c>
@@ -6348,23 +6376,23 @@
         <v>91</v>
       </c>
       <c r="F92">
-        <f>A92*100</f>
+        <f t="shared" si="8"/>
         <v>5.2749995142200001</v>
       </c>
       <c r="G92">
-        <f>B92*100</f>
+        <f t="shared" si="9"/>
         <v>6.3250005245200001</v>
       </c>
       <c r="H92">
-        <f>C92*100</f>
+        <f t="shared" si="10"/>
         <v>7.34999999404</v>
       </c>
       <c r="I92">
-        <f>D92*100</f>
+        <f t="shared" si="11"/>
         <v>9.1249994933600007</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>5.2749995142200003E-2</v>
       </c>
@@ -6381,23 +6409,23 @@
         <v>92</v>
       </c>
       <c r="F93">
-        <f>A93*100</f>
+        <f t="shared" si="8"/>
         <v>5.2749995142200001</v>
       </c>
       <c r="G93">
-        <f>B93*100</f>
+        <f t="shared" si="9"/>
         <v>6.3250005245200001</v>
       </c>
       <c r="H93">
-        <f>C93*100</f>
+        <f t="shared" si="10"/>
         <v>7.34999999404</v>
       </c>
       <c r="I93">
-        <f>D93*100</f>
+        <f t="shared" si="11"/>
         <v>9.09999907017</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>5.2749995142200003E-2</v>
       </c>
@@ -6414,23 +6442,23 @@
         <v>93</v>
       </c>
       <c r="F94">
-        <f>A94*100</f>
+        <f t="shared" si="8"/>
         <v>5.2749995142200001</v>
       </c>
       <c r="G94">
-        <f>B94*100</f>
+        <f t="shared" si="9"/>
         <v>6.3250005245200001</v>
       </c>
       <c r="H94">
-        <f>C94*100</f>
+        <f t="shared" si="10"/>
         <v>7.34999999404</v>
       </c>
       <c r="I94">
-        <f>D94*100</f>
+        <f t="shared" si="11"/>
         <v>9.09999907017</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>5.2749995142200003E-2</v>
       </c>
@@ -6447,23 +6475,23 @@
         <v>94</v>
       </c>
       <c r="F95">
-        <f>A95*100</f>
+        <f t="shared" si="8"/>
         <v>5.2749995142200001</v>
       </c>
       <c r="G95">
-        <f>B95*100</f>
+        <f t="shared" si="9"/>
         <v>6.3250005245200001</v>
       </c>
       <c r="H95">
-        <f>C95*100</f>
+        <f t="shared" si="10"/>
         <v>7.34999999404</v>
       </c>
       <c r="I95">
-        <f>D95*100</f>
+        <f t="shared" si="11"/>
         <v>9.09999907017</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>5.2749995142200003E-2</v>
       </c>
@@ -6480,23 +6508,23 @@
         <v>95</v>
       </c>
       <c r="F96">
-        <f>A96*100</f>
+        <f t="shared" si="8"/>
         <v>5.2749995142200001</v>
       </c>
       <c r="G96">
-        <f>B96*100</f>
+        <f t="shared" si="9"/>
         <v>6.3500002026600004</v>
       </c>
       <c r="H96">
-        <f>C96*100</f>
+        <f t="shared" si="10"/>
         <v>7.34999999404</v>
       </c>
       <c r="I96">
-        <f>D96*100</f>
+        <f t="shared" si="11"/>
         <v>9.09999907017</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>5.2749995142200003E-2</v>
       </c>
@@ -6513,23 +6541,23 @@
         <v>96</v>
       </c>
       <c r="F97">
-        <f>A97*100</f>
+        <f t="shared" si="8"/>
         <v>5.2749995142200001</v>
       </c>
       <c r="G97">
-        <f>B97*100</f>
+        <f t="shared" si="9"/>
         <v>6.3500002026600004</v>
       </c>
       <c r="H97">
-        <f>C97*100</f>
+        <f t="shared" si="10"/>
         <v>7.34999999404</v>
       </c>
       <c r="I97">
-        <f>D97*100</f>
+        <f t="shared" si="11"/>
         <v>9.0749986469700001</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>5.2749995142200003E-2</v>
       </c>
@@ -6546,23 +6574,23 @@
         <v>97</v>
       </c>
       <c r="F98">
-        <f>A98*100</f>
+        <f t="shared" si="8"/>
         <v>5.2749995142200001</v>
       </c>
       <c r="G98">
-        <f>B98*100</f>
+        <f t="shared" si="9"/>
         <v>6.3500002026600004</v>
       </c>
       <c r="H98">
-        <f>C98*100</f>
+        <f t="shared" si="10"/>
         <v>7.34999999404</v>
       </c>
       <c r="I98">
-        <f>D98*100</f>
+        <f t="shared" si="11"/>
         <v>9.09999907017</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>5.2749995142200003E-2</v>
       </c>
@@ -6579,23 +6607,23 @@
         <v>98</v>
       </c>
       <c r="F99">
-        <f>A99*100</f>
+        <f t="shared" si="8"/>
         <v>5.2749995142200001</v>
       </c>
       <c r="G99">
-        <f>B99*100</f>
+        <f t="shared" si="9"/>
         <v>6.3500002026600004</v>
       </c>
       <c r="H99">
-        <f>C99*100</f>
+        <f t="shared" si="10"/>
         <v>7.34999999404</v>
       </c>
       <c r="I99">
-        <f>D99*100</f>
+        <f t="shared" si="11"/>
         <v>9.1499991715000011</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>5.2749995142200003E-2</v>
       </c>
@@ -6612,23 +6640,23 @@
         <v>99</v>
       </c>
       <c r="F100">
-        <f>A100*100</f>
+        <f t="shared" si="8"/>
         <v>5.2749995142200001</v>
       </c>
       <c r="G100">
-        <f>B100*100</f>
+        <f t="shared" si="9"/>
         <v>6.3500002026600004</v>
       </c>
       <c r="H100">
-        <f>C100*100</f>
+        <f t="shared" si="10"/>
         <v>7.34999999404</v>
       </c>
       <c r="I100">
-        <f>D100*100</f>
+        <f t="shared" si="11"/>
         <v>9.0999998152300012</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>5.2749995142200003E-2</v>
       </c>
@@ -6645,23 +6673,23 @@
         <v>100</v>
       </c>
       <c r="F101">
-        <f>A101*100</f>
+        <f t="shared" si="8"/>
         <v>5.2749995142200001</v>
       </c>
       <c r="G101">
-        <f>B101*100</f>
+        <f t="shared" si="9"/>
         <v>6.3500002026600004</v>
       </c>
       <c r="H101">
-        <f>C101*100</f>
+        <f t="shared" si="10"/>
         <v>7.34999999404</v>
       </c>
       <c r="I101">
-        <f>D101*100</f>
+        <f t="shared" si="11"/>
         <v>9.0750001370900009</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>5.2749995142200003E-2</v>
       </c>
@@ -6678,23 +6706,23 @@
         <v>101</v>
       </c>
       <c r="F102">
-        <f>A102*100</f>
+        <f t="shared" si="8"/>
         <v>5.2749995142200001</v>
       </c>
       <c r="G102">
-        <f>B102*100</f>
+        <f t="shared" si="9"/>
         <v>6.3500002026600004</v>
       </c>
       <c r="H102">
-        <f>C102*100</f>
+        <f t="shared" si="10"/>
         <v>7.34999999404</v>
       </c>
       <c r="I102">
-        <f>D102*100</f>
+        <f t="shared" si="11"/>
         <v>9.0250007808199992</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B103">
         <v>6.35000020266E-2</v>
       </c>
@@ -6702,7 +6730,7 @@
         <v>7.3499999940400004E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B104">
         <v>6.35000020266E-2</v>
       </c>
@@ -6710,32 +6738,32 @@
         <v>7.3249995708499993E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C105">
         <v>7.3249995708499993E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C106">
         <v>7.3499999940400004E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C107">
         <v>7.3499999940400004E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C108">
         <v>7.3499999940400004E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C109">
         <v>7.3499999940400004E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C110">
         <v>7.3749996721700004E-2</v>
       </c>

</xml_diff>